<commit_message>
Adding few more test cases in the spreadsheet and logging
</commit_message>
<xml_diff>
--- a/ConsoleApplication1/ConsoleApplication1/bin/Debug/test.xlsx
+++ b/ConsoleApplication1/ConsoleApplication1/bin/Debug/test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8810" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9520" uniqueCount="97">
   <si>
     <t>Id</t>
   </si>
@@ -289,6 +289,24 @@
   </si>
   <si>
     <t>option150</t>
+  </si>
+  <si>
+    <t>https://emergenciesdev2.worldvision.com.au/#/disaster-ready-donate</t>
+  </si>
+  <si>
+    <t>option1000</t>
+  </si>
+  <si>
+    <t>option5000</t>
+  </si>
+  <si>
+    <t>option10000</t>
+  </si>
+  <si>
+    <t>Clear</t>
+  </si>
+  <si>
+    <t>https://emergenciesdev2.worldvision.com.au/#/typhoon-haiyan</t>
   </si>
 </sst>
 </file>
@@ -656,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD169"/>
+  <dimension ref="A1:XFD371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="C156" sqref="C156"/>
+    <sheetView tabSelected="1" topLeftCell="A328" workbookViewId="0">
+      <selection activeCell="C353" sqref="C353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27267,40 +27285,44 @@
         <v>89</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A153" s="3"/>
-      <c r="B153" s="3"/>
+    <row r="153" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="C153" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D153" s="5" t="s">
-        <v>89</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D153" s="5"/>
     </row>
     <row r="154" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B154" s="3" t="s">
-        <v>86</v>
+      <c r="B154" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D154" s="5"/>
-    </row>
-    <row r="155" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="D154" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B155" s="6" t="s">
-        <v>87</v>
+      <c r="B155" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D155" s="5" t="s">
-        <v>88</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
@@ -27308,13 +27330,13 @@
         <v>0</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C156" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D156" s="5" t="s">
-        <v>2</v>
+      <c r="D156" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -27322,13 +27344,13 @@
         <v>0</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C157" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D157" s="3" t="s">
-        <v>3</v>
+      <c r="D157" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -27336,13 +27358,13 @@
         <v>0</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D158" s="5" t="s">
-        <v>4</v>
+      <c r="D158" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -27350,13 +27372,13 @@
         <v>0</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C159" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -27364,39 +27386,39 @@
         <v>0</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>67</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D160" s="2"/>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D161" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C162" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>2</v>
+        <v>49</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -27404,13 +27426,13 @@
         <v>0</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -27418,13 +27440,13 @@
         <v>0</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -27432,13 +27454,13 @@
         <v>0</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
@@ -27446,49 +27468,2657 @@
         <v>0</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D166" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D166" s="2"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B167" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" s="3"/>
+      <c r="B168" s="3"/>
+      <c r="C168" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D168" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B169" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D169" s="5"/>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D170" s="5"/>
+    </row>
+    <row r="171" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D171" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D174" s="5"/>
+    </row>
+    <row r="175" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D180" s="2"/>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B186" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="C186" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D167" s="2"/>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="3" t="s">
+      <c r="D186" s="2"/>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B168" s="3" t="s">
+      <c r="B187" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C168" s="3" t="s">
+      <c r="C187" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D168" s="3" t="s">
+      <c r="D187" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A169" s="3"/>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D169" s="5" t="s">
-        <v>89</v>
+    <row r="188" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C188" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D188" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B189" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D189" s="5"/>
+    </row>
+    <row r="190" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D190" s="5"/>
+    </row>
+    <row r="191" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D191" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D194" s="5"/>
+    </row>
+    <row r="195" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C195" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D195" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C196" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C197" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D197" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C199" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D199" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D200" s="2"/>
+    </row>
+    <row r="201" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C201" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D201" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C202" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D202" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C203" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D203" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C204" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D204" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C205" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D205" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D206" s="2"/>
+    </row>
+    <row r="207" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C207" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D207" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C208" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D208" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B209" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C209" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D209" s="5"/>
+    </row>
+    <row r="210" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C211" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D211" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C212" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C213" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D213" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C214" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C215" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D215" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C216" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C217" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D217" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C218" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C219" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D219" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C220" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D220" s="2"/>
+    </row>
+    <row r="221" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C221" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D221" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C222" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D222" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C223" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D223" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C224" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D224" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C225" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D225" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C226" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D226" s="2"/>
+    </row>
+    <row r="227" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C227" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C228" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D228" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B229" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C229" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C230" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A231" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C231" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D231" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A232" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C232" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A233" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B233" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C233" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A234" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C234" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D234" s="5"/>
+    </row>
+    <row r="235" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A235" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C235" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D235" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A236" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C236" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A237" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C237" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D237" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A238" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C238" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A239" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C239" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D239" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A240" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C240" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D240" s="2"/>
+    </row>
+    <row r="241" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A241" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C241" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D241" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B242" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C242" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D242" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B243" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C243" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D243" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B244" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C244" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D244" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C245" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D245" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C246" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D246" s="2"/>
+    </row>
+    <row r="247" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B247" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C247" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D247" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C248" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D248" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B249" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C249" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D249" s="5"/>
+    </row>
+    <row r="250" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B250" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D250" s="5"/>
+    </row>
+    <row r="251" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B251" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C251" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D251" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C252" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D252" s="5"/>
+    </row>
+    <row r="253" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C253" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D253" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A254" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C254" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C255" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D255" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A256" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D256" s="5"/>
+    </row>
+    <row r="257" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A257" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C257" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D257" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A258" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B258" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C258" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A259" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B259" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C259" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D259" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A260" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B260" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C260" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A261" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B261" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D261" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A262" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D262" s="2"/>
+    </row>
+    <row r="263" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A263" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B263" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D263" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A264" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B264" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D264" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A265" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D265" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A266" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B266" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D266" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A267" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D267" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A268" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B268" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D268" s="2"/>
+    </row>
+    <row r="269" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A269" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C269" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D269" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" s="3"/>
+      <c r="B270" s="3"/>
+      <c r="C270" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D270" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B271" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C271" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D271" s="5"/>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B272" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C272" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D272" s="5"/>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C273" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D273" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B274" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C274" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C275" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D275" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C276" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D276" s="5"/>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C277" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D277" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C278" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C279" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D279" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B280" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C280" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D280" s="3"/>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B281" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C281" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D281" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D282" s="2"/>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C283" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D283" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C284" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D284" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C285" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D285" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B286" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C286" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D286" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C287" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D287" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C288" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D288" s="2"/>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B289" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C289" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D289" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" s="3"/>
+      <c r="B290" s="3"/>
+      <c r="C290" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D290" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C291" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D291" s="5"/>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B292" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C292" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D292" s="5"/>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B293" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C293" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D293" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C294" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C295" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D295" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C296" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D296" s="5"/>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C297" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D297" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B298" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C298" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B299" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C299" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D299" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B300" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C300" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B301" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C301" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D301" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B302" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C302" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D302" s="2"/>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B303" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C303" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D303" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C304" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D304" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C305" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D305" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B306" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C306" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D306" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B307" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C307" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D307" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B308" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C308" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D308" s="2"/>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D309" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A310" s="3"/>
+      <c r="B310" s="3"/>
+      <c r="C310" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D310" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C311" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D311" s="5"/>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C312" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D312" s="5"/>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B313" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C313" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D313" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B314" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C314" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B315" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C315" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D315" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B316" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C316" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D316" s="5"/>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B317" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C317" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D317" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C318" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A319" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C319" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D319" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B320" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C320" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D320" s="3"/>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C321" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D321" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A322" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B322" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C322" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D322" s="2"/>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A323" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C323" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D323" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A324" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C324" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D324" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A325" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B325" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C325" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D325" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A326" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B326" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C326" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D326" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A327" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B327" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C327" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D327" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A328" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B328" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C328" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D328" s="2"/>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A329" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C329" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D329" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A330" s="3"/>
+      <c r="B330" s="3"/>
+      <c r="C330" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D330" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C331" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D331" s="5"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C332" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D332" s="5"/>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C333" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D333" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A334" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B334" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C334" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D334" s="3"/>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A335" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B335" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C335" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D335" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A336" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B336" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C336" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D336" s="5"/>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A337" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B337" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C337" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D337" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A338" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B338" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C338" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D338" s="3"/>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A339" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C339" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D339" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="340" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A340" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B340" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C340" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D340" s="3"/>
+    </row>
+    <row r="341" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A341" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B341" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C341" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D341" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A342" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B342" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C342" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D342" s="2"/>
+    </row>
+    <row r="343" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A343" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B343" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C343" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D343" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A344" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C344" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D344" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="345" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A345" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B345" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C345" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D345" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="346" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A346" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B346" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C346" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D346" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="347" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A347" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B347" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C347" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D347" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="348" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A348" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B348" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C348" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D348" s="2"/>
+    </row>
+    <row r="349" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A349" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B349" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C349" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D349" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="350" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A350" s="3"/>
+      <c r="B350" s="3"/>
+      <c r="C350" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D350" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="351" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C351" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D351" s="5"/>
+    </row>
+    <row r="352" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C352" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D352" s="5"/>
+    </row>
+    <row r="353" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C353" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D353" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B354" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C354" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D354" s="5"/>
+    </row>
+    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B355" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C355" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D355" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B356" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C356" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D356" s="3"/>
+    </row>
+    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B357" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C357" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D357" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B358" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C358" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D358" s="5"/>
+    </row>
+    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A359" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B359" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C359" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D359" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A360" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C360" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D360" s="3"/>
+    </row>
+    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A361" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B361" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C361" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D361" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A362" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B362" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C362" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D362" s="3"/>
+    </row>
+    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A363" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B363" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C363" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D363" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A364" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C364" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D364" s="2"/>
+    </row>
+    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A365" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B365" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C365" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D365" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A366" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B366" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C366" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D366" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A367" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B367" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C367" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D367" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A368" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C368" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D368" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A369" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B369" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C369" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D369" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A370" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C370" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D370" s="2"/>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B371" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C371" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D371" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -31606,13 +34236,31 @@
     <hyperlink ref="D122" r:id="rId4111" location="/south-sudan-donate"/>
     <hyperlink ref="D141" r:id="rId4112"/>
     <hyperlink ref="D137" r:id="rId4113" location="/south-sudan-donate"/>
-    <hyperlink ref="D152" r:id="rId4114" location="/south-sudan-donate"/>
-    <hyperlink ref="D158" r:id="rId4115"/>
-    <hyperlink ref="D153" r:id="rId4116" location="/south-sudan-donate"/>
-    <hyperlink ref="D169" r:id="rId4117" location="/south-sudan-donate"/>
+    <hyperlink ref="D157" r:id="rId4114"/>
+    <hyperlink ref="D152" r:id="rId4115" location="/south-sudan-donate"/>
+    <hyperlink ref="D168" r:id="rId4116" location="/disaster-ready-donate"/>
+    <hyperlink ref="D175" r:id="rId4117"/>
+    <hyperlink ref="D188" r:id="rId4118" location="/disaster-ready-donate"/>
+    <hyperlink ref="D195" r:id="rId4119"/>
+    <hyperlink ref="D208" r:id="rId4120" location="/disaster-ready-donate"/>
+    <hyperlink ref="D228" r:id="rId4121" location="/disaster-ready-donate"/>
+    <hyperlink ref="D215" r:id="rId4122"/>
+    <hyperlink ref="D235" r:id="rId4123"/>
+    <hyperlink ref="D248" r:id="rId4124" location="/disaster-ready-donate"/>
+    <hyperlink ref="D257" r:id="rId4125"/>
+    <hyperlink ref="D270" r:id="rId4126" location="/typhoon-haiyan"/>
+    <hyperlink ref="D277" r:id="rId4127"/>
+    <hyperlink ref="D290" r:id="rId4128" location="/typhoon-haiyan"/>
+    <hyperlink ref="D297" r:id="rId4129"/>
+    <hyperlink ref="D310" r:id="rId4130" location="/typhoon-haiyan"/>
+    <hyperlink ref="D317" r:id="rId4131"/>
+    <hyperlink ref="D330" r:id="rId4132" location="/typhoon-haiyan"/>
+    <hyperlink ref="D337" r:id="rId4133"/>
+    <hyperlink ref="D350" r:id="rId4134" location="/typhoon-haiyan"/>
+    <hyperlink ref="D359" r:id="rId4135"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4118"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4136"/>
 </worksheet>
 </file>
 

</xml_diff>